<commit_message>
Chinh sua du lieu thu nghiem
</commit_message>
<xml_diff>
--- a/setup/DuLieuThuNghiem.xlsx
+++ b/setup/DuLieuThuNghiem.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thevi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HocPhan\DoAnCSN\csn-da22ttc-phamthevinh-vattunongnghiep\setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" tabRatio="744" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" tabRatio="744" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Nhóm sản phẩm" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="160">
   <si>
     <t>PG00001</t>
   </si>
@@ -136,9 +136,6 @@
     <t>Nam</t>
   </si>
   <si>
-    <t>0123456789</t>
-  </si>
-  <si>
     <t>Khóm 1, Phường 2, Tp Trà Vinh, Tỉnh Trà Vinh</t>
   </si>
   <si>
@@ -148,9 +145,6 @@
     <t>Nguyễn Văn Hoàng</t>
   </si>
   <si>
-    <t>0987654321</t>
-  </si>
-  <si>
     <t>Khóm 8, Phường 7, Tp Trà Vinh, Tỉnh Trà Vinh</t>
   </si>
   <si>
@@ -163,9 +157,6 @@
     <t>Nữ</t>
   </si>
   <si>
-    <t>0456123789</t>
-  </si>
-  <si>
     <t>Tư vấn &amp; bán hàng</t>
   </si>
   <si>
@@ -464,6 +455,57 @@
   </si>
   <si>
     <t>Lượng kali cây hấp thụ được, cải thiện chất lượng và tăng sức đề kháng.</t>
+  </si>
+  <si>
+    <t>B00003</t>
+  </si>
+  <si>
+    <t>PVCFC</t>
+  </si>
+  <si>
+    <t>info@pvcfc.com.vn</t>
+  </si>
+  <si>
+    <t>173 - 179 Trương Văn Bang, Phường Thạnh Mỹ Lợi, Thành phố Thủ Đức, Thành phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>B00004</t>
+  </si>
+  <si>
+    <t>JVF</t>
+  </si>
+  <si>
+    <t>info@jvf.com.vn</t>
+  </si>
+  <si>
+    <t>0290381900</t>
+  </si>
+  <si>
+    <t>0286290506</t>
+  </si>
+  <si>
+    <t>KCN Gò Dầu, Ấp 4, Xã Phước Thái, Huyện Long Thành, Tỉnh Đồng Nai</t>
+  </si>
+  <si>
+    <t>E00004</t>
+  </si>
+  <si>
+    <t>Trương Cẩm Tú</t>
+  </si>
+  <si>
+    <t>0986156324</t>
+  </si>
+  <si>
+    <t>0706895623</t>
+  </si>
+  <si>
+    <t>0831564785</t>
+  </si>
+  <si>
+    <t>0978624531</t>
+  </si>
+  <si>
+    <t>Khóm 2, Phường 4, Tp Trà Vinh, Tỉnh Trà Vinh</t>
   </si>
 </sst>
 </file>
@@ -475,7 +517,7 @@
     <numFmt numFmtId="165" formatCode="#.#%"/>
     <numFmt numFmtId="166" formatCode="#.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -492,6 +534,31 @@
     <font>
       <sz val="10"/>
       <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -537,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -578,6 +645,21 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -895,7 +977,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -908,16 +990,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -928,7 +1010,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>2</v>
@@ -942,7 +1024,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>5</v>
@@ -956,7 +1038,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>5</v>
@@ -970,7 +1052,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>2</v>
@@ -984,84 +1066,126 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F3"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" customWidth="1"/>
-    <col min="5" max="5" width="72" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" style="14" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" style="14" customWidth="1"/>
+    <col min="5" max="5" width="81" style="14" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" style="14" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="A1" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="16" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1089,34 +1213,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1142,7 +1266,7 @@
         <v>46069</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>13</v>
@@ -1174,7 +1298,7 @@
         <v>46069</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>13</v>
@@ -1206,7 +1330,7 @@
         <v>46069</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>13</v>
@@ -1238,7 +1362,7 @@
         <v>46069</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>13</v>
@@ -1270,7 +1394,7 @@
         <v>46069</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>23</v>
@@ -1286,10 +1410,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1306,25 +1430,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1340,14 +1464,14 @@
       <c r="D2" s="9">
         <v>35836</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1355,7 +1479,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>35</v>
@@ -1363,37 +1487,60 @@
       <c r="D3" s="9">
         <v>36800</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>40</v>
+      <c r="E3" s="13" t="s">
+        <v>156</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="D4" s="9">
         <v>36319</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>45</v>
+      <c r="E4" s="13" t="s">
+        <v>157</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="9">
+        <v>37025</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1419,90 +1566,90 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1528,90 +1675,90 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1623,7 +1770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -1637,27 +1784,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D2" s="10">
         <v>0.46</v>
@@ -1665,13 +1812,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D3" s="11">
         <v>1.2E-2</v>
@@ -1679,13 +1826,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D4" s="10">
         <v>0.01</v>
@@ -1693,13 +1840,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D5" s="10">
         <v>0.25</v>
@@ -1707,13 +1854,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D6" s="10">
         <v>0.01</v>
@@ -1721,13 +1868,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D7" s="12">
         <v>5.0000000000000001E-3</v>
@@ -1735,13 +1882,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D8" s="10">
         <v>0.12</v>
@@ -1749,13 +1896,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D9" s="10">
         <v>0.04</v>
@@ -1763,13 +1910,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D10" s="10">
         <v>0.18</v>
@@ -1777,13 +1924,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D11" s="10">
         <v>0.46</v>
@@ -1791,13 +1938,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D12" s="11">
         <v>2.5000000000000001E-2</v>
@@ -1805,27 +1952,27 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D14" s="10">
         <v>0.61</v>
@@ -1833,13 +1980,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D15" s="10">
         <v>0.01</v>
@@ -1867,123 +2014,123 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>